<commit_message>
RoundFill.SHORTEN_ALL always filled from west, needs to fill from loser's left for fair games; otherwise the round starter might be able to capture on opening moves. Comments removed from Bao, because they were wrong. Added comments to SHORTEN_ALL about assumed options and fairness. Better description in Bule_Perga. Removed round play from Depouiller. Added an ability to add parameter overrides for fairness experiments; see --params option.
</commit_message>
<xml_diff>
--- a/analysis/data/Final Combined Results.xlsx
+++ b/analysis/data/Final Combined Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5942D7A6-87FB-46F4-8AAD-E5DCF862E3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFA3398-96EB-4A40-90AE-E476581B6E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30945" yWindow="1860" windowWidth="25410" windowHeight="10785" xr2:uid="{8CFCA730-4EDD-4AF7-80E4-9848B77F6D14}"/>
+    <workbookView xWindow="31440" yWindow="1650" windowWidth="25410" windowHeight="14265" xr2:uid="{8CFCA730-4EDD-4AF7-80E4-9848B77F6D14}"/>
   </bookViews>
   <sheets>
     <sheet name="Fairness" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="183">
   <si>
     <t>LOOPED</t>
   </si>
@@ -605,6 +605,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>bug found and fixed (fill order must be dep. on loser)</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1121,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1150,6 +1153,8 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1771,11 +1776,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AI142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16:C16"/>
+      <selection pane="bottomRight" activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3288,63 +3293,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+    <row r="19" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>35</v>
       </c>
       <c r="B19">
-        <v>153</v>
+        <v>283</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F19">
-        <v>27993</v>
+        <v>21497</v>
       </c>
       <c r="G19">
-        <v>23899</v>
+        <v>28289</v>
       </c>
       <c r="H19">
-        <v>21934</v>
+        <v>28352</v>
       </c>
       <c r="I19">
-        <v>26017</v>
+        <v>21555</v>
       </c>
       <c r="J19">
-        <v>155</v>
-      </c>
-      <c r="K19">
-        <v>7640</v>
+        <v>285</v>
+      </c>
+      <c r="K19" s="15">
+        <v>22938</v>
       </c>
       <c r="L19">
-        <v>47951</v>
+        <v>49907</v>
       </c>
       <c r="M19">
-        <v>54010</v>
+        <v>43052</v>
       </c>
       <c r="N19" s="1">
-        <v>0.48026401450276934</v>
+        <v>0.50060686306962376</v>
       </c>
       <c r="O19" s="1">
-        <v>0.54094929038590589</v>
+        <v>0.4318457665031647</v>
       </c>
       <c r="P19" s="1">
-        <v>2.0000000000000002E-5</v>
+        <v>2.2000000000000001E-4</v>
       </c>
       <c r="Q19">
-        <v>1.0568863143784419E-35</v>
+        <v>0.70155346326168655</v>
       </c>
       <c r="R19">
-        <v>1.1699706079965645E-147</v>
+        <v>0</v>
       </c>
       <c r="S19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" t="b">
         <v>0</v>
@@ -3360,15 +3365,18 @@
       </c>
       <c r="AE19" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF19" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG19" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
@@ -4824,7 +4832,7 @@
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="16" t="s">
         <v>54</v>
       </c>
       <c r="B38">
@@ -4840,16 +4848,16 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>29887</v>
+        <v>72059</v>
       </c>
       <c r="G38">
-        <v>30609</v>
+        <v>78116</v>
       </c>
       <c r="H38">
-        <v>30113</v>
+        <v>77941</v>
       </c>
       <c r="I38">
-        <v>29391</v>
+        <v>71884</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -4858,28 +4866,28 @@
         <v>0</v>
       </c>
       <c r="L38">
-        <v>59504</v>
+        <v>149825</v>
       </c>
       <c r="M38">
-        <v>59278</v>
+        <v>143943</v>
       </c>
       <c r="N38" s="1">
-        <v>0.49586666666666668</v>
+        <v>0.49941666666666601</v>
       </c>
       <c r="O38" s="1">
-        <v>0.49398333333333333</v>
+        <v>0.47981000000000001</v>
       </c>
       <c r="P38" s="1">
         <v>0</v>
       </c>
       <c r="Q38">
-        <v>4.1878077707538782E-3</v>
+        <v>0.52281665391908805</v>
       </c>
       <c r="R38">
-        <v>3.0665253308703635E-5</v>
+        <v>2.1670277259777199E-108</v>
       </c>
       <c r="S38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T38" t="b">
         <v>0</v>
@@ -4887,7 +4895,7 @@
       <c r="V38" s="3"/>
       <c r="X38" s="4">
         <f t="shared" si="4"/>
-        <v>120000</v>
+        <v>300000</v>
       </c>
       <c r="AD38" t="b" cm="1">
         <f t="array" ref="AD38">OR(NOT(ISBLANK(Y38:AB38)))</f>
@@ -4895,15 +4903,15 @@
       </c>
       <c r="AE38" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF38" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG38" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI38" s="5" t="s">
         <v>181</v>
@@ -11304,55 +11312,57 @@
         <v>0</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F117">
-        <v>4954</v>
+        <v>29857</v>
       </c>
       <c r="G117">
-        <v>5009</v>
+        <v>30223</v>
       </c>
       <c r="H117">
-        <v>5046</v>
+        <v>30143</v>
       </c>
       <c r="I117">
-        <v>4991</v>
+        <v>29776</v>
       </c>
       <c r="J117">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="K117">
+        <v>18</v>
       </c>
       <c r="L117">
-        <v>10037</v>
+        <v>59919</v>
       </c>
       <c r="M117">
-        <v>9945</v>
+        <v>59633</v>
       </c>
       <c r="N117" s="1">
-        <v>0.50185000000000002</v>
+        <v>0.49932916107634229</v>
       </c>
       <c r="O117" s="1">
-        <v>0.49725000000000003</v>
+        <v>0.49694580788173237</v>
       </c>
       <c r="P117" s="1">
-        <v>0</v>
+        <v>8.3333333333333337E-6</v>
       </c>
       <c r="Q117">
-        <v>0.60079401595699999</v>
+        <v>0.64209695910600217</v>
       </c>
       <c r="R117">
-        <v>0.43667663367489001</v>
+        <v>3.4345015667030687E-2</v>
       </c>
       <c r="S117" t="b">
         <v>1</v>
       </c>
       <c r="T117" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V117" s="3"/>
       <c r="X117" s="4">
         <f t="shared" si="10"/>
-        <v>20000</v>
+        <v>120000</v>
       </c>
       <c r="AD117" t="b" cm="1">
         <f t="array" ref="AD117">OR(NOT(ISBLANK(Y117:AB117)))</f>
@@ -11368,7 +11378,7 @@
       </c>
       <c r="AG117" t="b">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI117" s="5" t="s">
         <v>181</v>

</xml_diff>

<commit_message>
Adji_Kui_II quitter config changed to hole_owner; game was not fair with seeds being divvied  (used on games that reach the ENDLESS condition). Corrected the implementation of ALLOW_RULE of OPP_OR_EMPTY, previously North's the check for enough seeds to sow a full half of the board was always checking the South side (wrong index was used). Boola, Dabuda, Depouiller, Gamacha, and Sadeqa were effected. Added Rounds.END_S_SEEDS and Rounds.END_2S_SEEDS conditions to skip NoOutcomeChange ender deco (it has not effect). All games now report Winner Fair in "Final Combined Results.xlsx".
</commit_message>
<xml_diff>
--- a/analysis/data/Final Combined Results.xlsx
+++ b/analysis/data/Final Combined Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8BE070-E3CA-4999-9580-48CA92C0D65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27642331-1D9A-4D21-A5D9-BD4E45140ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32055" yWindow="960" windowWidth="25410" windowHeight="14265" xr2:uid="{8CFCA730-4EDD-4AF7-80E4-9848B77F6D14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8CFCA730-4EDD-4AF7-80E4-9848B77F6D14}"/>
   </bookViews>
   <sheets>
     <sheet name="Fairness" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="187">
   <si>
     <t>LOOPED</t>
   </si>
@@ -559,9 +559,6 @@
   </si>
   <si>
     <t>20K</t>
-  </si>
-  <si>
-    <t>note added about variations that are fair</t>
   </si>
   <si>
     <t>Max Moves</t>
@@ -617,6 +614,12 @@
   </si>
   <si>
     <t>changed board size to 14, bugs in ender &amp; setup, 20K moves still isn't enough to finish most games</t>
+  </si>
+  <si>
+    <t>re-ran all 400K at once, something in other orig. raw data sets seemed wrong</t>
+  </si>
+  <si>
+    <t>bug found and fixed (wrong side of board checked for &gt;start seeds)</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -955,12 +958,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1124,7 +1121,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1155,7 +1152,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1203,37 +1204,7 @@
     <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="16" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1675,24 +1646,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA1143D-0630-44D1-88D2-0F6770CCC143}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AI142"/>
+  <dimension ref="A1:AI146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="9" width="11.7109375" customWidth="1"/>
-    <col min="19" max="20" width="10.5703125" customWidth="1"/>
+    <col min="19" max="20" width="12.85546875" customWidth="1"/>
     <col min="21" max="21" width="3.28515625" customWidth="1"/>
     <col min="22" max="22" width="11.7109375" customWidth="1"/>
     <col min="23" max="23" width="2.85546875" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1"/>
     <col min="25" max="27" width="8.5703125" style="4" customWidth="1"/>
     <col min="28" max="28" width="8.5703125" customWidth="1"/>
     <col min="29" max="29" width="4" customWidth="1"/>
@@ -1702,7 +1673,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1755,10 +1726,10 @@
       <c r="R1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="14" t="s">
         <v>17</v>
       </c>
       <c r="U1" s="6"/>
@@ -1770,10 +1741,10 @@
         <v>160</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AA1" s="5" t="s">
         <v>165</v>
@@ -1783,22 +1754,22 @@
       </c>
       <c r="AC1" s="2"/>
       <c r="AD1" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="AE1" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="AE1" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="AF1" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG1" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="AG1" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="AH1" s="6" t="s">
         <v>161</v>
       </c>
       <c r="AI1" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -1889,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>653</v>
+        <v>1293</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1898,43 +1869,43 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>47454</v>
+        <v>95351</v>
       </c>
       <c r="G3">
-        <v>51832</v>
+        <v>103863</v>
       </c>
       <c r="H3">
-        <v>52236</v>
+        <v>104007</v>
       </c>
       <c r="I3">
-        <v>47825</v>
+        <v>95486</v>
       </c>
       <c r="J3">
-        <v>653</v>
+        <v>1293</v>
       </c>
       <c r="K3">
-        <v>337</v>
+        <v>732</v>
       </c>
       <c r="L3">
-        <v>100061</v>
+        <v>199493</v>
       </c>
       <c r="M3">
-        <v>95279</v>
+        <v>190837</v>
       </c>
       <c r="N3" s="1">
-        <v>0.50194384665934277</v>
+        <v>0.5003498809903012</v>
       </c>
       <c r="O3" s="1">
-        <v>0.47795552478843423</v>
+        <v>0.47863970283942847</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>8.2601207409401009E-2</v>
+        <v>0.65859597708944362</v>
       </c>
       <c r="R3">
-        <v>2.9014619341057253E-86</v>
+        <v>2.8909799829062444E-160</v>
       </c>
       <c r="S3" t="b">
         <v>1</v>
@@ -1945,7 +1916,7 @@
       <c r="V3" s="3"/>
       <c r="X3" s="11">
         <f t="shared" si="0"/>
-        <v>200000</v>
+        <v>400000</v>
       </c>
       <c r="AD3" t="b" cm="1">
         <f t="array" ref="AD3">OR(NOT(ISBLANK(Y3:AB3)))</f>
@@ -1953,15 +1924,15 @@
       </c>
       <c r="AE3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF3" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -2131,67 +2102,70 @@
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="16" t="s">
         <v>23</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>1799</v>
+        <v>3322</v>
       </c>
       <c r="D6">
-        <v>607</v>
+        <v>592</v>
       </c>
       <c r="E6">
-        <v>625</v>
+        <v>610</v>
       </c>
       <c r="F6">
-        <v>23724</v>
+        <v>38297</v>
       </c>
       <c r="G6">
-        <v>23903</v>
+        <v>39337</v>
       </c>
       <c r="H6">
-        <v>24787</v>
+        <v>39455</v>
       </c>
       <c r="I6">
-        <v>24554</v>
+        <v>38384</v>
+      </c>
+      <c r="J6">
+        <v>3325</v>
       </c>
       <c r="K6">
-        <v>1800</v>
+        <v>37495</v>
       </c>
       <c r="L6">
-        <v>49341</v>
+        <v>77839</v>
       </c>
       <c r="M6">
-        <v>48278</v>
+        <v>76681</v>
       </c>
       <c r="N6" s="1">
-        <v>0.50883796716442542</v>
+        <v>0.50065927845992553</v>
       </c>
       <c r="O6" s="1">
-        <v>0.4978755878227869</v>
+        <v>0.49321103985901088</v>
       </c>
       <c r="P6" s="1">
-        <v>1.2319999999999999E-2</v>
+        <v>7.5125000000000001E-3</v>
       </c>
       <c r="Q6">
-        <v>3.7078455008636148E-8</v>
+        <v>0.60312780643192332</v>
       </c>
       <c r="R6">
-        <v>0.18581192312018263</v>
+        <v>8.613426948866934E-8</v>
       </c>
       <c r="S6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" s="3"/>
       <c r="X6" s="11">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>160000</v>
       </c>
       <c r="AD6" t="b" cm="1">
         <f t="array" ref="AD6">OR(NOT(ISBLANK(Y6:AB6)))</f>
@@ -2199,18 +2173,18 @@
       </c>
       <c r="AE6" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6" t="b">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -3058,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="AH16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
@@ -3310,7 +3284,7 @@
         <v>0</v>
       </c>
       <c r="AH19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -3567,49 +3541,49 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>25490</v>
+        <v>50507</v>
       </c>
       <c r="G23">
-        <v>24525</v>
+        <v>49513</v>
       </c>
       <c r="H23">
-        <v>24510</v>
+        <v>49491</v>
       </c>
       <c r="I23">
-        <v>25471</v>
+        <v>50486</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L23">
-        <v>49981</v>
+        <v>99977</v>
       </c>
       <c r="M23">
-        <v>50961</v>
+        <v>100993</v>
       </c>
       <c r="N23" s="1">
-        <v>0.49982999319972798</v>
+        <v>0.49989249838747501</v>
       </c>
       <c r="O23" s="1">
-        <v>0.5096303852154086</v>
+        <v>0.504972574588618</v>
       </c>
       <c r="P23" s="1">
-        <v>4.0000000000000003E-5</v>
+        <v>1.5E-5</v>
       </c>
       <c r="Q23">
-        <v>0.914376784154593</v>
+        <v>0.92340013515705799</v>
       </c>
       <c r="R23">
-        <v>1.1244010474630665E-9</v>
+        <v>8.6846125563766299E-6</v>
       </c>
       <c r="S23" t="b">
         <v>1</v>
@@ -3620,7 +3594,7 @@
       <c r="V23" s="3"/>
       <c r="X23" s="11">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="AD23" t="b" cm="1">
         <f t="array" ref="AD23">OR(NOT(ISBLANK(Y23:AB23)))</f>
@@ -3640,7 +3614,7 @@
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B24">
@@ -3650,49 +3624,49 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>1027</v>
+        <v>1352</v>
       </c>
       <c r="E24">
-        <v>1023</v>
+        <v>1364</v>
       </c>
       <c r="F24">
-        <v>78847</v>
+        <v>104944</v>
       </c>
       <c r="G24">
-        <v>70599</v>
+        <v>94153</v>
       </c>
       <c r="H24">
-        <v>70126</v>
+        <v>93704</v>
       </c>
       <c r="I24">
-        <v>78378</v>
+        <v>104483</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="L24">
-        <v>148504</v>
+        <v>198187</v>
       </c>
       <c r="M24">
-        <v>157225</v>
+        <v>209427</v>
       </c>
       <c r="N24" s="1">
-        <v>0.49841919785198857</v>
+        <v>0.4988547235730611</v>
       </c>
       <c r="O24" s="1">
-        <v>0.52768920959892596</v>
+        <v>0.52714682695502457</v>
       </c>
       <c r="P24" s="1">
-        <v>6.8333333333333336E-3</v>
+        <v>6.79E-3</v>
       </c>
       <c r="Q24">
-        <v>8.4391450322844494E-2</v>
+        <v>0.14881037983875264</v>
       </c>
       <c r="R24">
-        <v>1.0094466069505381E-200</v>
+        <v>1.1563026646017995E-256</v>
       </c>
       <c r="S24" t="b">
         <v>1</v>
@@ -3703,7 +3677,7 @@
       <c r="V24" s="3"/>
       <c r="X24" s="11">
         <f t="shared" si="0"/>
-        <v>300000</v>
+        <v>400000</v>
       </c>
       <c r="Z24" s="4" t="s">
         <v>159</v>
@@ -3792,7 +3766,7 @@
         <v>100000</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AD25" t="b" cm="1">
         <f t="array" ref="AD25">OR(NOT(ISBLANK(Y25:AB25)))</f>
@@ -3811,7 +3785,7 @@
         <v>1</v>
       </c>
       <c r="AH25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
@@ -4480,55 +4454,55 @@
         <v>45</v>
       </c>
       <c r="B34">
-        <v>2546</v>
+        <v>4963</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>5187</v>
+        <v>10360</v>
       </c>
       <c r="E34">
-        <v>5139</v>
+        <v>10396</v>
       </c>
       <c r="F34">
-        <v>45733</v>
+        <v>91996</v>
       </c>
       <c r="G34">
-        <v>47463</v>
+        <v>94760</v>
       </c>
       <c r="H34">
-        <v>47780</v>
+        <v>95116</v>
       </c>
       <c r="I34">
-        <v>46152</v>
+        <v>92409</v>
       </c>
       <c r="J34">
-        <v>2546</v>
+        <v>4963</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
-        <v>93932</v>
+        <v>187525</v>
       </c>
       <c r="M34">
-        <v>91885</v>
+        <v>184405</v>
       </c>
       <c r="N34" s="1">
-        <v>0.50196656833824971</v>
+        <v>0.50102730301564868</v>
       </c>
       <c r="O34" s="1">
-        <v>0.49102753195673549</v>
+        <v>0.49269132015784933</v>
       </c>
       <c r="P34" s="1">
-        <v>5.1630000000000002E-2</v>
+        <v>5.1889999999999999E-2</v>
       </c>
       <c r="Q34">
-        <v>8.8866432569111975E-2</v>
+        <v>0.20876184035093007</v>
       </c>
       <c r="R34">
-        <v>8.3157684950246883E-15</v>
+        <v>3.7983495870430142E-19</v>
       </c>
       <c r="S34" t="b">
         <v>1</v>
@@ -4539,7 +4513,7 @@
       <c r="V34" s="3"/>
       <c r="X34" s="11">
         <f t="shared" ref="X34:X65" si="4">SUM(B34:I34)</f>
-        <v>200000</v>
+        <v>400000</v>
       </c>
       <c r="AD34" t="b" cm="1">
         <f t="array" ref="AD34">OR(NOT(ISBLANK(Y34:AB34)))</f>
@@ -4547,19 +4521,22 @@
       </c>
       <c r="AE34" t="b">
         <f t="shared" ref="AE34:AE65" si="5">OR(NOT(S34),AND(Q34&gt;0.05, Q34&lt;0.15), P34&gt;0.1,O34&gt;0.6, O34&lt;0.4,L34&lt;8000,(C34/X34)&gt;0.05, (B34/X34)&gt;0.05)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF34" t="b">
         <f t="shared" ref="AF34:AF65" si="6">OR(NOT(S34), AND(Q34&gt;0.05, Q34&lt;0.15), L34&lt;8000,(C34/X34)&gt;0.05, (B34/X34)&gt;0.05)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG34" t="b">
         <f t="shared" ref="AG34:AG65" si="7">OR(AND(Q34&lt;=0.15, Q34&gt;0.001), AND(R34&lt;=0.15, R34&gt;0.001))</f>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" t="s">
         <v>51</v>
       </c>
       <c r="B35">
@@ -4569,49 +4546,52 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>2293</v>
+        <v>4608</v>
       </c>
       <c r="E35">
-        <v>2232</v>
+        <v>4640</v>
       </c>
       <c r="F35">
-        <v>23033</v>
+        <v>46599</v>
       </c>
       <c r="G35">
-        <v>24082</v>
+        <v>48692</v>
       </c>
       <c r="H35">
-        <v>24674</v>
+        <v>48793</v>
       </c>
       <c r="I35">
-        <v>23686</v>
+        <v>46668</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
       </c>
       <c r="K35">
-        <v>0</v>
+        <v>389</v>
       </c>
       <c r="L35">
-        <v>48360</v>
+        <v>95461</v>
       </c>
       <c r="M35">
-        <v>46719</v>
+        <v>93267</v>
       </c>
       <c r="N35" s="1">
-        <v>0.50652003142183821</v>
+        <v>0.500445604764301</v>
       </c>
       <c r="O35" s="1">
-        <v>0.48933228593872741</v>
+        <v>0.488943759436336</v>
       </c>
       <c r="P35" s="1">
-        <v>4.5249999999999999E-2</v>
+        <v>4.6240000000000003E-2</v>
       </c>
       <c r="Q35">
-        <v>5.5954417347355195E-5</v>
+        <v>0.69710066643549295</v>
       </c>
       <c r="R35">
-        <v>4.3265563304719134E-11</v>
+        <v>4.5615299440872502E-22</v>
       </c>
       <c r="S35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T35" t="b">
         <v>0</v>
@@ -4619,7 +4599,7 @@
       <c r="V35" s="3"/>
       <c r="X35" s="11">
         <f t="shared" si="4"/>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="AD35" t="b" cm="1">
         <f t="array" ref="AD35">OR(NOT(ISBLANK(Y35:AB35)))</f>
@@ -4627,18 +4607,18 @@
       </c>
       <c r="AE35" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF35" t="b">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG35" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AH35" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
@@ -4824,16 +4804,16 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>72059</v>
+        <v>48175</v>
       </c>
       <c r="G38">
-        <v>78116</v>
+        <v>51831</v>
       </c>
       <c r="H38">
-        <v>77941</v>
+        <v>51825</v>
       </c>
       <c r="I38">
-        <v>71884</v>
+        <v>48169</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -4842,25 +4822,25 @@
         <v>0</v>
       </c>
       <c r="L38">
-        <v>149825</v>
+        <v>99994</v>
       </c>
       <c r="M38">
-        <v>143943</v>
+        <v>96344</v>
       </c>
       <c r="N38" s="1">
-        <v>0.49941666666666601</v>
+        <v>0.49997000000000003</v>
       </c>
       <c r="O38" s="1">
-        <v>0.47981000000000001</v>
+        <v>0.48171999999999998</v>
       </c>
       <c r="P38" s="1">
         <v>0</v>
       </c>
       <c r="Q38">
-        <v>0.52281665391908805</v>
+        <v>0.97859307946745</v>
       </c>
       <c r="R38">
-        <v>2.1670277259777199E-108</v>
+        <v>4.34059766599125E-60</v>
       </c>
       <c r="S38" t="b">
         <v>1</v>
@@ -4871,7 +4851,7 @@
       <c r="V38" s="3"/>
       <c r="X38" s="11">
         <f t="shared" si="4"/>
-        <v>300000</v>
+        <v>200000</v>
       </c>
       <c r="AD38" t="b" cm="1">
         <f t="array" ref="AD38">OR(NOT(ISBLANK(Y38:AB38)))</f>
@@ -4890,7 +4870,7 @@
         <v>0</v>
       </c>
       <c r="AH38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
@@ -5820,43 +5800,43 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F50">
-        <v>28450</v>
+        <v>56747</v>
       </c>
       <c r="G50">
-        <v>21652</v>
+        <v>43117</v>
       </c>
       <c r="H50">
-        <v>21550</v>
+        <v>43253</v>
       </c>
       <c r="I50">
-        <v>28348</v>
+        <v>56880</v>
       </c>
       <c r="J50">
         <v>0</v>
       </c>
       <c r="K50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L50">
-        <v>49898</v>
+        <v>100133</v>
       </c>
       <c r="M50">
-        <v>56798</v>
+        <v>113627</v>
       </c>
       <c r="N50" s="1">
-        <v>0.49897999999999998</v>
+        <v>0.50067251008765101</v>
       </c>
       <c r="O50" s="1">
-        <v>0.56798000000000004</v>
+        <v>0.56814352215283204</v>
       </c>
       <c r="P50" s="1">
-        <v>0</v>
+        <v>1.5E-5</v>
       </c>
       <c r="Q50">
-        <v>0.51885937542701055</v>
+        <v>0.54750248584183503</v>
       </c>
       <c r="R50">
         <v>0</v>
@@ -5870,7 +5850,7 @@
       <c r="V50" s="3"/>
       <c r="X50" s="11">
         <f t="shared" si="4"/>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="AD50" t="b" cm="1">
         <f t="array" ref="AD50">OR(NOT(ISBLANK(Y50:AB50)))</f>
@@ -7380,7 +7360,7 @@
         <v>0</v>
       </c>
       <c r="AH68" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.25">
@@ -7450,7 +7430,7 @@
         <v>100000</v>
       </c>
       <c r="Y69" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AD69" t="b" cm="1">
         <f t="array" ref="AD69">OR(NOT(ISBLANK(Y69:AB69)))</f>
@@ -7619,7 +7599,7 @@
         <v>200000</v>
       </c>
       <c r="Y71" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AD71" t="b" cm="1">
         <f t="array" ref="AD71">OR(NOT(ISBLANK(Y71:AB71)))</f>
@@ -8056,7 +8036,7 @@
         <v>0</v>
       </c>
       <c r="AH76" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.25">
@@ -8805,7 +8785,7 @@
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -10121,7 +10101,7 @@
         <v>160000</v>
       </c>
       <c r="Y101" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AD101" t="b" cm="1">
         <f t="array" ref="AD101">OR(NOT(ISBLANK(Y101:AB101)))</f>
@@ -10140,11 +10120,11 @@
         <v>0</v>
       </c>
       <c r="AH101" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="102" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B102">
@@ -10154,49 +10134,49 @@
         <v>0</v>
       </c>
       <c r="D102">
-        <v>2197</v>
+        <v>3294</v>
       </c>
       <c r="E102">
-        <v>2125</v>
+        <v>3203</v>
       </c>
       <c r="F102">
-        <v>50358</v>
+        <v>75466</v>
       </c>
       <c r="G102">
-        <v>47095</v>
+        <v>70895</v>
       </c>
       <c r="H102">
-        <v>47445</v>
+        <v>71240</v>
       </c>
       <c r="I102">
-        <v>50780</v>
+        <v>75902</v>
       </c>
       <c r="J102">
         <v>0</v>
       </c>
       <c r="K102">
-        <v>404</v>
+        <v>621</v>
       </c>
       <c r="L102">
-        <v>98225</v>
+        <v>147142</v>
       </c>
       <c r="M102">
-        <v>101138</v>
+        <v>151368</v>
       </c>
       <c r="N102" s="1">
-        <v>0.50197262850192659</v>
+        <v>0.50133048043801942</v>
       </c>
       <c r="O102" s="1">
-        <v>0.51685933012397922</v>
+        <v>0.51572897040234678</v>
       </c>
       <c r="P102" s="1">
-        <v>2.1610000000000001E-2</v>
+        <v>2.1656666666666668E-2</v>
       </c>
       <c r="Q102">
-        <v>8.0949295158554702E-2</v>
+        <v>0.1494152597887862</v>
       </c>
       <c r="R102">
-        <v>2.6084305119683916E-50</v>
+        <v>3.9650737633623318E-65</v>
       </c>
       <c r="S102" t="b">
         <v>1</v>
@@ -10207,7 +10187,7 @@
       <c r="V102" s="3"/>
       <c r="X102" s="11">
         <f t="shared" si="13"/>
-        <v>200000</v>
+        <v>300000</v>
       </c>
       <c r="Z102" s="4" t="s">
         <v>159</v>
@@ -10564,55 +10544,55 @@
         <v>122</v>
       </c>
       <c r="B107">
-        <v>5512</v>
+        <v>7437</v>
       </c>
       <c r="C107">
-        <v>583</v>
+        <v>762</v>
       </c>
       <c r="D107">
-        <v>7561</v>
+        <v>10080</v>
       </c>
       <c r="E107">
-        <v>7638</v>
+        <v>10162</v>
       </c>
       <c r="F107">
-        <v>67521</v>
+        <v>90107</v>
       </c>
       <c r="G107">
-        <v>71402</v>
+        <v>95438</v>
       </c>
       <c r="H107">
-        <v>71958</v>
+        <v>95755</v>
       </c>
       <c r="I107">
-        <v>67825</v>
+        <v>90259</v>
       </c>
       <c r="J107">
-        <v>6095</v>
+        <v>8199</v>
       </c>
       <c r="K107">
         <v>0</v>
       </c>
       <c r="L107">
-        <v>139783</v>
+        <v>186014</v>
       </c>
       <c r="M107">
-        <v>135346</v>
+        <v>180366</v>
       </c>
       <c r="N107" s="1">
-        <v>0.50154284443104924</v>
+        <v>0.50063112453203928</v>
       </c>
       <c r="O107" s="1">
-        <v>0.48562284270880424</v>
+        <v>0.48543030851089597</v>
       </c>
       <c r="P107" s="1">
-        <v>5.0663333333333331E-2</v>
+        <v>5.0604999999999997E-2</v>
       </c>
       <c r="Q107">
-        <v>0.1033096778122488</v>
+        <v>0.44164877273502223</v>
       </c>
       <c r="R107">
-        <v>4.7865626954805242E-52</v>
+        <v>1.3894439975011013E-70</v>
       </c>
       <c r="S107" t="b">
         <v>1</v>
@@ -10623,7 +10603,7 @@
       <c r="V107" s="3"/>
       <c r="X107" s="11">
         <f t="shared" si="13"/>
-        <v>300000</v>
+        <v>400000</v>
       </c>
       <c r="AD107" t="b" cm="1">
         <f t="array" ref="AD107">OR(NOT(ISBLANK(Y107:AB107)))</f>
@@ -10631,15 +10611,15 @@
       </c>
       <c r="AE107" t="b">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF107" t="b">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG107" t="b">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:34" x14ac:dyDescent="0.25">
@@ -11418,60 +11398,60 @@
         <v>0</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E117">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F117">
-        <v>29857</v>
+        <v>49798</v>
       </c>
       <c r="G117">
-        <v>30223</v>
+        <v>50109</v>
       </c>
       <c r="H117">
-        <v>30143</v>
+        <v>50199</v>
       </c>
       <c r="I117">
-        <v>29776</v>
+        <v>49886</v>
       </c>
       <c r="J117">
         <v>0</v>
       </c>
       <c r="K117">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="L117">
-        <v>59919</v>
+        <v>100085</v>
       </c>
       <c r="M117">
-        <v>59633</v>
+        <v>99684</v>
       </c>
       <c r="N117" s="1">
-        <v>0.49932916107634229</v>
+        <v>0.50044501780071204</v>
       </c>
       <c r="O117" s="1">
-        <v>0.49694580788173237</v>
+        <v>0.49843993759750299</v>
       </c>
       <c r="P117" s="1">
-        <v>8.3333333333333337E-6</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="Q117">
-        <v>0.64209695910600217</v>
+        <v>0.69060950157477996</v>
       </c>
       <c r="R117">
-        <v>3.4345015667030687E-2</v>
+        <v>0.162915045818225</v>
       </c>
       <c r="S117" t="b">
         <v>1</v>
       </c>
       <c r="T117" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V117" s="3"/>
       <c r="X117" s="11">
         <f t="shared" si="13"/>
-        <v>120000</v>
+        <v>200000</v>
       </c>
       <c r="AD117" t="b" cm="1">
         <f t="array" ref="AD117">OR(NOT(ISBLANK(Y117:AB117)))</f>
@@ -11487,7 +11467,7 @@
       </c>
       <c r="AG117" t="b">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:33" x14ac:dyDescent="0.25">
@@ -13577,62 +13557,54 @@
         <v>0</v>
       </c>
     </row>
+    <row r="146" spans="24:24" x14ac:dyDescent="0.25">
+      <c r="X146" s="15"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AI142" xr:uid="{9FA1143D-0630-44D1-88D2-0F6770CCC143}"/>
   <conditionalFormatting sqref="L2:L142">
-    <cfRule type="cellIs" dxfId="13" priority="176" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="176" operator="lessThan">
       <formula>8000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:O142">
-    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>0.6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.48</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
       <formula>0.52</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P142">
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="18" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="19" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="19" stopIfTrue="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="20" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:R142">
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="15" operator="between">
       <formula>0.05</formula>
       <formula>0.15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="16" operator="between">
       <formula>0.001</formula>
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:T142">
-    <cfRule type="cellIs" dxfId="3" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
       <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X142">
-    <cfRule type="cellIs" dxfId="2" priority="9" stopIfTrue="1" operator="lessThan">
-      <formula>60000</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" stopIfTrue="1" operator="greaterThanOrEqual">
-      <formula>100000</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" stopIfTrue="1" operator="greaterThanOrEqual">
-      <formula>60000</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed man_profile.py to work. Attempted to improved the option handling in exper_config.py; it's still bad. Specified ender and quitter in the Game menu options.
</commit_message>
<xml_diff>
--- a/analysis/data/Final Combined Results.xlsx
+++ b/analysis/data/Final Combined Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27642331-1D9A-4D21-A5D9-BD4E45140ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C6F4AB-988E-49C9-BCF6-21409B836608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8CFCA730-4EDD-4AF7-80E4-9848B77F6D14}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8CFCA730-4EDD-4AF7-80E4-9848B77F6D14}"/>
   </bookViews>
   <sheets>
     <sheet name="Fairness" sheetId="1" r:id="rId1"/>
@@ -570,9 +570,6 @@
     <t>Bad Outcome</t>
   </si>
   <si>
-    <t>note added about variation that is fair</t>
-  </si>
-  <si>
     <t>Game</t>
   </si>
   <si>
@@ -586,9 +583,6 @@
 End</t>
   </si>
   <si>
-    <t>note added about ways add capture last 4/8 seeds</t>
-  </si>
-  <si>
     <t>20k</t>
   </si>
   <si>
@@ -620,6 +614,12 @@
   </si>
   <si>
     <t>bug found and fixed (wrong side of board checked for &gt;start seeds)</t>
+  </si>
+  <si>
+    <t>quitter config changed to make fair</t>
+  </si>
+  <si>
+    <t>note added about ways to capture last 4/8 seeds</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1121,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1156,7 +1156,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1204,7 +1203,15 @@
     <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="16" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1648,11 +1655,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AI146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="T144" sqref="T144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,7 +1680,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1744,7 +1751,7 @@
         <v>167</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AA1" s="5" t="s">
         <v>165</v>
@@ -1760,16 +1767,16 @@
         <v>169</v>
       </c>
       <c r="AF1" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG1" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="AG1" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="AH1" s="6" t="s">
         <v>161</v>
       </c>
       <c r="AI1" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -2102,7 +2109,7 @@
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6">
@@ -2184,7 +2191,7 @@
         <v>0</v>
       </c>
       <c r="AH6" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -3032,7 +3039,7 @@
         <v>1</v>
       </c>
       <c r="AH16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
@@ -3284,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="AH19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -3766,7 +3773,7 @@
         <v>100000</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AD25" t="b" cm="1">
         <f t="array" ref="AD25">OR(NOT(ISBLANK(Y25:AB25)))</f>
@@ -3785,7 +3792,7 @@
         <v>1</v>
       </c>
       <c r="AH25" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
@@ -4532,7 +4539,7 @@
         <v>0</v>
       </c>
       <c r="AH34" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
@@ -4618,7 +4625,7 @@
         <v>0</v>
       </c>
       <c r="AH35" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
@@ -4870,7 +4877,7 @@
         <v>0</v>
       </c>
       <c r="AH38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
@@ -7360,7 +7367,7 @@
         <v>0</v>
       </c>
       <c r="AH68" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.25">
@@ -7430,7 +7437,7 @@
         <v>100000</v>
       </c>
       <c r="Y69" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AD69" t="b" cm="1">
         <f t="array" ref="AD69">OR(NOT(ISBLANK(Y69:AB69)))</f>
@@ -7599,7 +7606,7 @@
         <v>200000</v>
       </c>
       <c r="Y71" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AD71" t="b" cm="1">
         <f t="array" ref="AD71">OR(NOT(ISBLANK(Y71:AB71)))</f>
@@ -8036,7 +8043,7 @@
         <v>0</v>
       </c>
       <c r="AH76" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.25">
@@ -8785,7 +8792,7 @@
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -10101,7 +10108,7 @@
         <v>160000</v>
       </c>
       <c r="Y101" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AD101" t="b" cm="1">
         <f t="array" ref="AD101">OR(NOT(ISBLANK(Y101:AB101)))</f>
@@ -10120,7 +10127,7 @@
         <v>0</v>
       </c>
       <c r="AH101" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:34" x14ac:dyDescent="0.25">
@@ -13563,47 +13570,47 @@
   </sheetData>
   <autoFilter ref="A1:AI142" xr:uid="{9FA1143D-0630-44D1-88D2-0F6770CCC143}"/>
   <conditionalFormatting sqref="L2:L142">
-    <cfRule type="cellIs" dxfId="10" priority="176" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="176" operator="lessThan">
       <formula>8000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:O142">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>0.6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.48</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>0.52</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P142">
-    <cfRule type="cellIs" dxfId="5" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="19" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="19" stopIfTrue="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="20" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:R142">
-    <cfRule type="cellIs" dxfId="2" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="between">
       <formula>0.05</formula>
       <formula>0.15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="16" operator="between">
       <formula>0.001</formula>
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:T142">
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="17" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>